<commit_message>
Verif fonction utilisée debloquée
</commit_message>
<xml_diff>
--- a/Quete/Taverne1.xlsx
+++ b/Quete/Taverne1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81922BD3-DAAC-4675-A2F5-7695009978D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFFD794-D4E0-45D6-B7AC-117B0AF6CE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
+    <workbookView xWindow="5760" yWindow="348" windowWidth="17280" windowHeight="9420" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="97" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,7 +643,7 @@
     </row>
     <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="3" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="4" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>

</xml_diff>